<commit_message>
#167 adding ui ureateam improvement
</commit_message>
<xml_diff>
--- a/src/main/data/IPLTeams.xlsx
+++ b/src/main/data/IPLTeams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/repo/Sport-fantasy-league/src/main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7A0DA06-719E-8F4A-B35C-8DD6A2671C61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E7E656-2EFE-E84E-A5FF-D7DD1DC721D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AEDD6B20-5EB6-CA43-852B-86DA822C2EF4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16220" xr2:uid="{AEDD6B20-5EB6-CA43-852B-86DA822C2EF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>DD</t>
   </si>
   <si>
-    <t>Delhi Daredevils</t>
-  </si>
-  <si>
     <t>INDIA</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>SUN TV Network</t>
+  </si>
+  <si>
+    <t>Delhi Capitals</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,10 +493,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -507,10 +507,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -521,10 +521,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -535,10 +535,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -549,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -563,10 +563,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
@@ -577,10 +577,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
@@ -588,13 +588,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
#195 adding banner and all logo changes , excel upload for player amtch schedule
</commit_message>
<xml_diff>
--- a/src/main/data/IPLTeams.xlsx
+++ b/src/main/data/IPLTeams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/repo/Sport-fantasy-league/src/main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E7E656-2EFE-E84E-A5FF-D7DD1DC721D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B179A8D4-422B-8F41-9F01-332579F15512}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16220" xr2:uid="{AEDD6B20-5EB6-CA43-852B-86DA822C2EF4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{AEDD6B20-5EB6-CA43-852B-86DA822C2EF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>